<commit_message>
reformat rule-based and goal-oriented chatbot
</commit_message>
<xml_diff>
--- a/data/babi/babi.xlsx
+++ b/data/babi/babi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="174">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -167,6 +167,9 @@
     <t xml:space="preserve">You are welcome.</t>
   </si>
   <si>
+    <t xml:space="preserve">fallback</t>
+  </si>
+  <si>
     <t xml:space="preserve">entity_name</t>
   </si>
   <si>
@@ -549,17 +552,106 @@
   </si>
   <si>
     <t xml:space="preserve">return {'BOOK_CUISINE': 'DONE!'}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">return {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">RESPONSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">helllooooo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M\月D\日"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -581,6 +673,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -625,7 +723,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -639,6 +737,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -661,8 +763,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,6 +1026,14 @@
       </c>
       <c r="F13" s="0" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -962,19 +1072,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>39</v>
@@ -982,27 +1092,27 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,16 +1120,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,13 +1151,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,10 +1165,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,10 +1176,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,10 +1187,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,10 +1198,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,10 +1209,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,10 +1220,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,10 +1231,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,10 +1242,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,10 +1253,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,10 +1264,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,10 +1275,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,10 +1286,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,10 +1297,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,10 +1308,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,10 +1319,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,10 +1330,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,10 +1341,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,10 +1352,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,10 +1363,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,7 +1374,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,7 +1382,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1390,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,7 +1398,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1296,7 +1406,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,7 +1414,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,7 +1422,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,272 +1430,272 @@
         <v>30</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1604,33 +1714,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="74.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="0" t="s">
         <v>171</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated rule based chatbot
</commit_message>
<xml_diff>
--- a/data/babi/babi.xlsx
+++ b/data/babi/babi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="173">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">action</t>
   </si>
   <si>
-    <t xml:space="preserve">2-5,7</t>
+    <t xml:space="preserve">0-7</t>
   </si>
   <si>
     <t xml:space="preserve">CUISINE,LOCATION,PARTY_SIZE,REST_TYPE,REST_INFO,BOOK_CUISINE </t>
@@ -60,11 +60,31 @@
 Hello, may I help you</t>
   </si>
   <si>
+    <t xml:space="preserve">1-7</t>
+  </si>
+  <si>
     <t xml:space="preserve">PARTY_SIZE,BOOK_CUISINE</t>
   </si>
   <si>
-    <t xml:space="preserve">may i have a table
-can you book a table</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">a table </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">with 5 people in tokyo for chinese food in cheap range</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">How many people would be in your party?</t>
@@ -79,9 +99,6 @@
     <t xml:space="preserve">LOCATION,BOOK_CUISINE</t>
   </si>
   <si>
-    <t xml:space="preserve">may i have a table</t>
-  </si>
-  <si>
     <t xml:space="preserve">Where should it be?</t>
   </si>
   <si>
@@ -91,26 +108,15 @@
     <t xml:space="preserve">Which price range are looking for?</t>
   </si>
   <si>
-    <t xml:space="preserve">7-12</t>
-  </si>
-  <si>
     <t xml:space="preserve">CUISINE,LOCATION,PARTY_SIZE,REST_TYPE,REST_INFO</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">it's perfect
-i love that
-that looks great</t>
-  </si>
-  <si>
     <t xml:space="preserve">Great! let me do the reservation.</t>
   </si>
   <si>
-    <t xml:space="preserve">6,8-11</t>
-  </si>
-  <si>
     <t xml:space="preserve">CUISINE,LOCATION,PARTY_SIZE,REST_TYPE</t>
   </si>
   <si>
@@ -121,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">getrestinfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-11</t>
   </si>
   <si>
     <t xml:space="preserve">no
@@ -138,9 +147,6 @@
     <t xml:space="preserve">Sure. Let me find an other option for you. What do you think of this option : {REST_INFO}</t>
   </si>
   <si>
-    <t xml:space="preserve">6,8-12</t>
-  </si>
-  <si>
     <t xml:space="preserve">REST_INFO,BOOK_CUISINE</t>
   </si>
   <si>
@@ -154,7 +160,13 @@
     <t xml:space="preserve">REST_INFO</t>
   </si>
   <si>
-    <t xml:space="preserve">thanks</t>
+    <t xml:space="preserve">thanks
+That looks great
+Fantastic
+Great
+let’s do it
+that’s great
+Sounds good</t>
   </si>
   <si>
     <t xml:space="preserve">Is there anything i can help you with?</t>
@@ -165,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">You are welcome.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset</t>
   </si>
   <si>
     <t xml:space="preserve">fallback</t>
@@ -570,6 +585,7 @@
         <color rgb="FF000000"/>
         <rFont val="新細明體"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'</t>
     </r>
@@ -589,6 +605,7 @@
         <color rgb="FF000000"/>
         <rFont val="新細明體"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'</t>
     </r>
@@ -608,6 +625,7 @@
         <color rgb="FF000000"/>
         <rFont val="新細明體"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'</t>
     </r>
@@ -627,6 +645,7 @@
         <color rgb="FF000000"/>
         <rFont val="新細明體"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'</t>
     </r>
@@ -641,6 +660,78 @@
       <t xml:space="preserve">}</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">return {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">SESSION_RESET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -651,7 +742,7 @@
     <numFmt numFmtId="165" formatCode="M\月D\日"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -679,6 +770,13 @@
       <color rgb="FF000000"/>
       <name val="新細明體"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -763,16 +861,16 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.96"/>
@@ -819,115 +917,115 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,22 +1033,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,22 +1056,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,36 +1079,36 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,13 +1117,16 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,7 +1134,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1056,7 +1157,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1072,47 +1173,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,16 +1221,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,13 +1238,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,13 +1252,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,10 +1277,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,10 +1299,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,10 +1310,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,10 +1321,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,10 +1332,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,10 +1343,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,10 +1354,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,10 +1365,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,10 +1376,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,10 +1387,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,10 +1398,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,10 +1409,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,10 +1420,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,10 +1431,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,10 +1442,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,10 +1453,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,10 +1464,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,7 +1475,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,7 +1483,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,7 +1491,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1499,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,7 +1507,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,7 +1515,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,7 +1523,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,272 +1531,272 @@
         <v>30</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1714,10 +1815,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1729,26 +1830,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for interact with goal response
</commit_message>
<xml_diff>
--- a/data/babi/babi.xlsx
+++ b/data/babi/babi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dialogs" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="170">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-7</t>
   </si>
   <si>
     <t xml:space="preserve">CUISINE,LOCATION,PARTY_SIZE,REST_TYPE,REST_INFO,BOOK_CUISINE </t>
@@ -58,9 +55,6 @@
   <si>
     <t xml:space="preserve">Hello, what can i help you with today?
 Hello, may I help you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-7</t>
   </si>
   <si>
     <t xml:space="preserve">PARTY_SIZE,BOOK_CUISINE</t>
@@ -128,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">getrestinfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-11</t>
   </si>
   <si>
     <t xml:space="preserve">no
@@ -871,8 +862,8 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -914,211 +905,178 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,16 +1085,16 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1123,7 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -1182,47 +1140,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,16 +1188,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,13 +1205,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,13 +1219,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,10 +1233,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,10 +1244,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,10 +1255,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,10 +1266,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,10 +1277,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,10 +1288,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,10 +1299,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,10 +1310,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,10 +1321,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,10 +1332,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,10 +1343,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,10 +1354,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,10 +1365,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,10 +1376,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,10 +1387,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,10 +1398,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,10 +1409,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,10 +1420,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,10 +1431,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1442,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,7 +1450,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1458,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1466,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1474,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,7 +1482,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,7 +1490,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,272 +1498,272 @@
         <v>30</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1839,34 +1797,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>